<commit_message>
working gui prototype connected with scraper
</commit_message>
<xml_diff>
--- a/Sketch-Sheet.xlsx
+++ b/Sketch-Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python\eHRAF_Scraper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericchantland/Documents/GitHub/eHRAF_Scraper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27268DE4-DBEE-4607-8306-A5603CFCC310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25092621-ABB2-514F-AE81-3DEAC25A25C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="30" windowWidth="19890" windowHeight="14055" activeTab="1" xr2:uid="{F516CA90-DCEB-E944-9429-AD1A28B6E802}"/>
+    <workbookView xWindow="62300" yWindow="3820" windowWidth="28480" windowHeight="21360" xr2:uid="{F516CA90-DCEB-E944-9429-AD1A28B6E802}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="67">
   <si>
     <t>?q=+-text%3Agalligaford</t>
   </si>
@@ -235,13 +235,19 @@
   </si>
   <si>
     <t>(subjects:( -"arranging a marriage"  -"gestures and signs") AND text:(Apple AND pear AND banana))</t>
+  </si>
+  <si>
+    <t>"</t>
+  </si>
+  <si>
+    <t>%22</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -632,20 +638,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87A14323-E30E-054C-9D2E-D98BCB6A2B31}">
-  <dimension ref="B1:K34"/>
+  <dimension ref="B1:K35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G27" sqref="G27:I34"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="100.875" customWidth="1"/>
+    <col min="6" max="6" width="100.83203125" customWidth="1"/>
     <col min="8" max="8" width="23" customWidth="1"/>
-    <col min="9" max="9" width="31.625" customWidth="1"/>
+    <col min="9" max="9" width="31.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="6:11">
+    <row r="1" spans="6:11" x14ac:dyDescent="0.2">
       <c r="F1" t="s">
         <v>40</v>
       </c>
@@ -662,7 +668,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="6:11">
+    <row r="3" spans="6:11" x14ac:dyDescent="0.2">
       <c r="F3" s="1" t="s">
         <v>0</v>
       </c>
@@ -676,7 +682,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="6:11">
+    <row r="4" spans="6:11" x14ac:dyDescent="0.2">
       <c r="F4" s="1" t="s">
         <v>1</v>
       </c>
@@ -690,7 +696,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="6:11">
+    <row r="5" spans="6:11" x14ac:dyDescent="0.2">
       <c r="F5" s="1" t="s">
         <v>2</v>
       </c>
@@ -701,7 +707,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="6:11" ht="31.5">
+    <row r="6" spans="6:11" ht="34" x14ac:dyDescent="0.2">
       <c r="F6" s="3" t="s">
         <v>25</v>
       </c>
@@ -718,7 +724,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="6:11" ht="33.950000000000003" customHeight="1">
+    <row r="7" spans="6:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F7" s="3" t="s">
         <v>31</v>
       </c>
@@ -729,12 +735,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="6:11">
+    <row r="8" spans="6:11" x14ac:dyDescent="0.2">
       <c r="F8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="6:11">
+    <row r="9" spans="6:11" x14ac:dyDescent="0.2">
       <c r="F9" t="s">
         <v>38</v>
       </c>
@@ -742,7 +748,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="2:8">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B27" s="9" t="s">
         <v>15</v>
       </c>
@@ -756,7 +762,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="2:8">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>10</v>
       </c>
@@ -776,7 +782,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="2:8">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>12</v>
       </c>
@@ -796,7 +802,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="2:8">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
       <c r="G32" t="s">
         <v>33</v>
       </c>
@@ -804,7 +810,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="7:9">
+    <row r="33" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G33" t="s">
         <v>24</v>
       </c>
@@ -812,7 +818,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="7:9" ht="20.25">
+    <row r="34" spans="7:9" ht="19" x14ac:dyDescent="0.2">
       <c r="G34" s="4" t="s">
         <v>27</v>
       </c>
@@ -821,6 +827,14 @@
       </c>
       <c r="I34" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G35" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H35" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -835,23 +849,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9357F785-3C4F-8149-BD12-06C9AF3A0403}">
   <dimension ref="H1:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="65.625" customWidth="1"/>
-    <col min="13" max="13" width="14.875" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="65.6640625" customWidth="1"/>
+    <col min="13" max="13" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="8:18">
+    <row r="1" spans="8:18" x14ac:dyDescent="0.2">
       <c r="H1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="8:18">
+    <row r="2" spans="8:18" x14ac:dyDescent="0.2">
       <c r="H2" t="s">
         <v>54</v>
       </c>
@@ -886,7 +900,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="8:18">
+    <row r="3" spans="8:18" x14ac:dyDescent="0.2">
       <c r="H3" t="s">
         <v>59</v>
       </c>
@@ -915,7 +929,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="8:18">
+    <row r="4" spans="8:18" x14ac:dyDescent="0.2">
       <c r="H4" t="s">
         <v>62</v>
       </c>
@@ -926,7 +940,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="8:18">
+    <row r="5" spans="8:18" x14ac:dyDescent="0.2">
       <c r="H5" t="s">
         <v>63</v>
       </c>
@@ -937,48 +951,48 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="8:18">
+    <row r="6" spans="8:18" x14ac:dyDescent="0.2">
       <c r="I6" s="4" t="s">
         <v>46</v>
       </c>
       <c r="J6" s="4"/>
     </row>
-    <row r="7" spans="8:18">
+    <row r="7" spans="8:18" x14ac:dyDescent="0.2">
       <c r="I7" s="4" t="s">
         <v>46</v>
       </c>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="8:18">
+    <row r="8" spans="8:18" x14ac:dyDescent="0.2">
       <c r="I8" s="4" t="s">
         <v>46</v>
       </c>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="8:18">
+    <row r="9" spans="8:18" x14ac:dyDescent="0.2">
       <c r="I9" s="4" t="s">
         <v>46</v>
       </c>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="8:18">
+    <row r="10" spans="8:18" x14ac:dyDescent="0.2">
       <c r="I10" s="4" t="s">
         <v>46</v>
       </c>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="8:18">
+    <row r="11" spans="8:18" x14ac:dyDescent="0.2">
       <c r="I11" s="4" t="s">
         <v>46</v>
       </c>
       <c r="J11" s="4"/>
     </row>
-    <row r="24" spans="13:15">
+    <row r="24" spans="13:15" x14ac:dyDescent="0.2">
       <c r="M24" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="13:15">
+    <row r="25" spans="13:15" x14ac:dyDescent="0.2">
       <c r="M25" s="2" t="s">
         <v>18</v>
       </c>
@@ -986,7 +1000,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="13:15">
+    <row r="26" spans="13:15" x14ac:dyDescent="0.2">
       <c r="M26" s="2" t="s">
         <v>17</v>
       </c>
@@ -994,7 +1008,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="13:15">
+    <row r="27" spans="13:15" x14ac:dyDescent="0.2">
       <c r="M27" t="s">
         <v>13</v>
       </c>
@@ -1002,7 +1016,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="13:15">
+    <row r="28" spans="13:15" x14ac:dyDescent="0.2">
       <c r="M28" t="s">
         <v>57</v>
       </c>
@@ -1010,7 +1024,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="13:15">
+    <row r="30" spans="13:15" x14ac:dyDescent="0.2">
       <c r="M30" t="s">
         <v>33</v>
       </c>
@@ -1018,7 +1032,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="13:15">
+    <row r="31" spans="13:15" x14ac:dyDescent="0.2">
       <c r="M31" t="s">
         <v>24</v>
       </c>
@@ -1026,7 +1040,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="13:15" ht="20.25">
+    <row r="32" spans="13:15" ht="19" x14ac:dyDescent="0.2">
       <c r="M32" s="4" t="s">
         <v>27</v>
       </c>

</xml_diff>